<commit_message>
Updated with 2019 calibration results and correctly transcripted manual readings.
</commit_message>
<xml_diff>
--- a/indResults.xlsx
+++ b/indResults.xlsx
@@ -1264,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>-23</v>
+        <v>-21</v>
       </c>
       <c r="F13" t="n">
         <v>1591</v>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>1.257071024723325e-06</v>
+        <v>1.257071024688318e-06</v>
       </c>
       <c r="W13" t="n">
-        <v>0.01257071024925347</v>
+        <v>0.01257071024856734</v>
       </c>
     </row>
     <row r="14">
@@ -1375,19 +1375,19 @@
         <v>0.1039164240377833</v>
       </c>
       <c r="Q14" t="n">
-        <v>9.17121500753135e-06</v>
+        <v>9.171214630206793e-06</v>
       </c>
       <c r="R14" t="n">
-        <v>2.01536703317403</v>
+        <v>2.015367043532096</v>
       </c>
       <c r="S14" t="n">
-        <v>167.5710476473234</v>
+        <v>167.5690475035215</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9940252045329921</v>
+        <v>0.9940193103620883</v>
       </c>
       <c r="U14" t="n">
-        <v>2.083732002920048</v>
+        <v>2.083731978016969</v>
       </c>
       <c r="V14" t="n">
         <v>1.929981878828665e-06</v>
@@ -1450,19 +1450,19 @@
         <v>0.2077338276609196</v>
       </c>
       <c r="Q15" t="n">
-        <v>1.683849088607998e-05</v>
+        <v>1.683849059714099e-05</v>
       </c>
       <c r="R15" t="n">
-        <v>2.037546967064912</v>
+        <v>2.037546973570641</v>
       </c>
       <c r="S15" t="n">
-        <v>243.023472356516</v>
+        <v>243.0214722127141</v>
       </c>
       <c r="T15" t="n">
-        <v>1.441701892574915</v>
+        <v>1.441695999039852</v>
       </c>
       <c r="U15" t="n">
-        <v>2.08370177997248</v>
+        <v>2.083701762568274</v>
       </c>
       <c r="V15" t="n">
         <v>3.177629941913367e-06</v>
@@ -1525,19 +1525,19 @@
         <v>0.3043857540059706</v>
       </c>
       <c r="Q16" t="n">
-        <v>2.427293667268685e-05</v>
+        <v>2.42729364272612e-05</v>
       </c>
       <c r="R16" t="n">
-        <v>2.043793889877027</v>
+        <v>2.043793894106823</v>
       </c>
       <c r="S16" t="n">
-        <v>300.3885966655541</v>
+        <v>300.3865965217523</v>
       </c>
       <c r="T16" t="n">
-        <v>1.78249563409863</v>
+        <v>1.782489742283523</v>
       </c>
       <c r="U16" t="n">
-        <v>2.083520326249251</v>
+        <v>2.083520311005623</v>
       </c>
       <c r="V16" t="n">
         <v>4.453086766584074e-06</v>
@@ -1600,19 +1600,19 @@
         <v>0.3990512708208321</v>
       </c>
       <c r="Q17" t="n">
-        <v>3.162897494552097e-05</v>
+        <v>3.162897472755116e-05</v>
       </c>
       <c r="R17" t="n">
-        <v>2.046341457667924</v>
+        <v>2.046341460664965</v>
       </c>
       <c r="S17" t="n">
-        <v>349.0250934233068</v>
+        <v>349.023093279505</v>
       </c>
       <c r="T17" t="n">
-        <v>2.071750279993229</v>
+        <v>2.071744390105576</v>
       </c>
       <c r="U17" t="n">
-        <v>2.083308435693779</v>
+        <v>2.083308421409329</v>
       </c>
       <c r="V17" t="n">
         <v>5.737024115558409e-06</v>
@@ -1675,19 +1675,19 @@
         <v>0.4948800274562426</v>
       </c>
       <c r="Q18" t="n">
-        <v>3.910707538807167e-05</v>
+        <v>3.910707518920017e-05</v>
       </c>
       <c r="R18" t="n">
-        <v>2.047644348123878</v>
+        <v>2.047644350379364</v>
       </c>
       <c r="S18" t="n">
-        <v>394.557367000584</v>
+        <v>394.5553668567821</v>
       </c>
       <c r="T18" t="n">
-        <v>2.342761914819239</v>
+        <v>2.342756026865681</v>
       </c>
       <c r="U18" t="n">
-        <v>2.083094038071669</v>
+        <v>2.083094024397489</v>
       </c>
       <c r="V18" t="n">
         <v>7.052482419320692e-06</v>
@@ -1750,19 +1750,19 @@
         <v>0.5925971734134042</v>
       </c>
       <c r="Q19" t="n">
-        <v>4.674936296196576e-05</v>
+        <v>4.674936277754227e-05</v>
       </c>
       <c r="R19" t="n">
-        <v>2.048399378920762</v>
+        <v>2.048399380690509</v>
       </c>
       <c r="S19" t="n">
-        <v>437.9354857032657</v>
+        <v>437.9334855594639</v>
       </c>
       <c r="T19" t="n">
-        <v>2.601152925948738</v>
+        <v>2.601147039928809</v>
       </c>
       <c r="U19" t="n">
-        <v>2.082879205250917</v>
+        <v>2.082879191998188</v>
       </c>
       <c r="V19" t="n">
         <v>8.402475305058465e-06</v>
@@ -1825,19 +1825,19 @@
         <v>0.6901292812219834</v>
       </c>
       <c r="Q20" t="n">
-        <v>5.438697520888296e-05</v>
+        <v>5.438697503563156e-05</v>
       </c>
       <c r="R20" t="n">
-        <v>2.048865988391389</v>
+        <v>2.048865989830586</v>
       </c>
       <c r="S20" t="n">
-        <v>478.9904373800954</v>
+        <v>478.9884372362936</v>
       </c>
       <c r="T20" t="n">
-        <v>2.845876398675031</v>
+        <v>2.84587051452481</v>
       </c>
       <c r="U20" t="n">
-        <v>2.082671673995392</v>
+        <v>2.082671661058268</v>
       </c>
       <c r="V20" t="n">
         <v>9.755009411884262e-06</v>
@@ -1900,19 +1900,19 @@
         <v>0.7834945299657239</v>
       </c>
       <c r="Q21" t="n">
-        <v>6.170413443723847e-05</v>
+        <v>6.170413427237478e-05</v>
       </c>
       <c r="R21" t="n">
-        <v>2.049163716194592</v>
+        <v>2.049163717407181</v>
       </c>
       <c r="S21" t="n">
-        <v>517.3831976566593</v>
+        <v>517.3811975128574</v>
       </c>
       <c r="T21" t="n">
-        <v>3.07483061964939</v>
+        <v>3.074824737175694</v>
       </c>
       <c r="U21" t="n">
-        <v>2.082486185954812</v>
+        <v>2.08248617330185</v>
       </c>
       <c r="V21" t="n">
         <v>1.105283538809727e-05</v>
@@ -1975,19 +1975,19 @@
         <v>0.8787681721553864</v>
       </c>
       <c r="Q22" t="n">
-        <v>6.917481728604213e-05</v>
+        <v>6.917481712816919e-05</v>
       </c>
       <c r="R22" t="n">
-        <v>2.049377591723657</v>
+        <v>2.049377592762813</v>
       </c>
       <c r="S22" t="n">
-        <v>555.6319475794895</v>
+        <v>555.6299474356877</v>
       </c>
       <c r="T22" t="n">
-        <v>3.303023119326032</v>
+        <v>3.303017238470463</v>
       </c>
       <c r="U22" t="n">
-        <v>2.082307733137943</v>
+        <v>2.082307720752961</v>
       </c>
       <c r="V22" t="n">
         <v>1.237928491224566e-05</v>
@@ -2050,19 +2050,19 @@
         <v>0.9856512078077428</v>
       </c>
       <c r="Q23" t="n">
-        <v>7.755907110642203e-05</v>
+        <v>7.755907095531116e-05</v>
       </c>
       <c r="R23" t="n">
-        <v>2.049550019553041</v>
+        <v>2.049550020442524</v>
       </c>
       <c r="S23" t="n">
-        <v>596.4718837976202</v>
+        <v>596.4698836538183</v>
       </c>
       <c r="T23" t="n">
-        <v>3.546849207788059</v>
+        <v>3.546843328729151</v>
       </c>
       <c r="U23" t="n">
-        <v>2.082110108699112</v>
+        <v>2.082110096542589</v>
       </c>
       <c r="V23" t="n">
         <v>1.386908815699293e-05</v>

</xml_diff>